<commit_message>
Updated the Gant Chart and Project plan accurately reflect what has changed and the adjusted timeline we've followed
</commit_message>
<xml_diff>
--- a/Assignment2/SydneyGantt.xlsx
+++ b/Assignment2/SydneyGantt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Software Tech\Assignment\2810ICT_Assignment_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Magev\OneDrive\Desktop\Test\2810ICT_Assignment_1\Assignment2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F57FEEE6-0D22-4E85-AE46-A27F334AF001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF572446-4C21-4541-BF71-07DFEA49D600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="81">
   <si>
     <t>PERIODS</t>
   </si>
@@ -260,9 +260,6 @@
     <t>Identify cleanliness related words</t>
   </si>
   <si>
-    <t>Quantify frequency  of keywords</t>
-  </si>
-  <si>
     <t>Display data visually</t>
   </si>
   <si>
@@ -328,9 +325,6 @@
   </si>
   <si>
     <t>3.6.2</t>
-  </si>
-  <si>
-    <t>3.6.3</t>
   </si>
   <si>
     <t>3.7.1</t>
@@ -472,7 +466,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -529,6 +523,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -725,7 +725,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -744,7 +744,7 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="7">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -855,21 +855,12 @@
     <xf numFmtId="9" fontId="5" fillId="9" borderId="8" xfId="6" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="3" fontId="9" fillId="0" borderId="10" xfId="3" applyBorder="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -906,15 +897,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="12">
       <alignment vertical="center"/>
     </xf>
@@ -926,6 +908,15 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -950,26 +941,6 @@
     <cellStyle name="Title" xfId="8" builtinId="15" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="9">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="7"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1081,6 +1052,26 @@
         <bottom style="thin">
           <color theme="0"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="7"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
   </dxfs>
@@ -1329,8 +1320,8 @@
   </sheetPr>
   <dimension ref="A1:BO54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection sqref="A1:BD53"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A39" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="BD52" sqref="A1:BD52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1349,7 +1340,7 @@
   <sheetData>
     <row r="1" spans="1:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
       <c r="B1" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -1358,51 +1349,51 @@
       <c r="G1" s="9"/>
     </row>
     <row r="2" spans="1:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
       <c r="G2" s="5" t="s">
         <v>5</v>
       </c>
       <c r="H2" s="11">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="J2" s="12"/>
-      <c r="K2" s="53" t="s">
+      <c r="K2" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="55"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="52"/>
       <c r="P2" s="13"/>
-      <c r="Q2" s="53" t="s">
+      <c r="Q2" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="R2" s="56"/>
-      <c r="S2" s="56"/>
-      <c r="T2" s="55"/>
+      <c r="R2" s="53"/>
+      <c r="S2" s="53"/>
+      <c r="T2" s="52"/>
       <c r="U2" s="14"/>
-      <c r="V2" s="57" t="s">
-        <v>2</v>
-      </c>
-      <c r="W2" s="58"/>
-      <c r="X2" s="58"/>
-      <c r="Y2" s="59"/>
+      <c r="V2" s="54" t="s">
+        <v>2</v>
+      </c>
+      <c r="W2" s="55"/>
+      <c r="X2" s="55"/>
+      <c r="Y2" s="56"/>
       <c r="Z2" s="15"/>
-      <c r="AA2" s="60" t="s">
+      <c r="AA2" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="AB2" s="61"/>
-      <c r="AC2" s="61"/>
-      <c r="AD2" s="61"/>
-      <c r="AE2" s="61"/>
-      <c r="AF2" s="61"/>
-      <c r="AG2" s="62"/>
+      <c r="AB2" s="55"/>
+      <c r="AC2" s="55"/>
+      <c r="AD2" s="55"/>
+      <c r="AE2" s="55"/>
+      <c r="AF2" s="55"/>
+      <c r="AG2" s="56"/>
       <c r="AH2" s="16"/>
       <c r="AI2" s="18" t="s">
         <v>4</v>
@@ -1416,22 +1407,22 @@
       <c r="AP2" s="19"/>
     </row>
     <row r="3" spans="1:67" s="8" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="66" t="s">
+      <c r="C3" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="66" t="s">
+      <c r="D3" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="66" t="s">
+      <c r="E3" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="66" t="s">
+      <c r="F3" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="51" t="s">
+      <c r="G3" s="48" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="17" t="s">
@@ -1458,12 +1449,12 @@
       <c r="AA3" s="7"/>
     </row>
     <row r="4" spans="1:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="65"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1608,7 +1599,7 @@
       <c r="BC4" s="3">
         <v>48</v>
       </c>
-      <c r="BD4" s="45">
+      <c r="BD4" s="43">
         <v>49</v>
       </c>
       <c r="BE4" s="3">
@@ -1646,7 +1637,7 @@
       </c>
     </row>
     <row r="5" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="50">
+      <c r="A5" s="47">
         <v>1</v>
       </c>
       <c r="B5" s="21" t="s">
@@ -1667,7 +1658,7 @@
       <c r="G5" s="36">
         <v>0</v>
       </c>
-      <c r="BD5" s="46"/>
+      <c r="BD5" s="44"/>
     </row>
     <row r="6" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="22">
@@ -1691,7 +1682,7 @@
       <c r="G6" s="32">
         <v>0</v>
       </c>
-      <c r="BD6" s="46"/>
+      <c r="BD6" s="44"/>
     </row>
     <row r="7" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="22">
@@ -1715,7 +1706,7 @@
       <c r="G7" s="32">
         <v>0</v>
       </c>
-      <c r="BD7" s="46"/>
+      <c r="BD7" s="44"/>
     </row>
     <row r="8" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="22">
@@ -1739,7 +1730,7 @@
       <c r="G8" s="32">
         <v>0</v>
       </c>
-      <c r="BD8" s="46"/>
+      <c r="BD8" s="44"/>
     </row>
     <row r="9" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="22">
@@ -1754,12 +1745,16 @@
       <c r="D9" s="33">
         <v>49</v>
       </c>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
+      <c r="E9" s="33">
+        <v>1</v>
+      </c>
+      <c r="F9" s="33">
+        <v>49</v>
+      </c>
       <c r="G9" s="32">
         <v>0</v>
       </c>
-      <c r="BD9" s="46"/>
+      <c r="BD9" s="44"/>
     </row>
     <row r="10" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22">
@@ -1783,7 +1778,7 @@
       <c r="G10" s="32">
         <v>0</v>
       </c>
-      <c r="BD10" s="46"/>
+      <c r="BD10" s="44"/>
     </row>
     <row r="11" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22">
@@ -1807,7 +1802,7 @@
       <c r="G11" s="32">
         <v>0</v>
       </c>
-      <c r="BD11" s="46"/>
+      <c r="BD11" s="44"/>
     </row>
     <row r="12" spans="1:67" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20">
@@ -1822,12 +1817,16 @@
       <c r="D12" s="35">
         <v>14</v>
       </c>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
+      <c r="E12" s="35">
+        <v>10</v>
+      </c>
+      <c r="F12" s="35">
+        <v>7</v>
+      </c>
       <c r="G12" s="36">
         <v>0</v>
       </c>
-      <c r="BD12" s="46"/>
+      <c r="BD12" s="44"/>
     </row>
     <row r="13" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22">
@@ -1842,12 +1841,16 @@
       <c r="D13" s="33">
         <v>1</v>
       </c>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
+      <c r="E13" s="33">
+        <v>10</v>
+      </c>
+      <c r="F13" s="33">
+        <v>1</v>
+      </c>
       <c r="G13" s="32">
         <v>0</v>
       </c>
-      <c r="BD13" s="46"/>
+      <c r="BD13" s="44"/>
     </row>
     <row r="14" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22">
@@ -1862,12 +1865,16 @@
       <c r="D14" s="33">
         <v>1</v>
       </c>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
+      <c r="E14" s="33">
+        <v>10</v>
+      </c>
+      <c r="F14" s="33">
+        <v>2</v>
+      </c>
       <c r="G14" s="32">
         <v>0</v>
       </c>
-      <c r="BD14" s="46"/>
+      <c r="BD14" s="44"/>
     </row>
     <row r="15" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22">
@@ -1882,12 +1889,16 @@
       <c r="D15" s="33">
         <v>1</v>
       </c>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
+      <c r="E15" s="33">
+        <v>10</v>
+      </c>
+      <c r="F15" s="33">
+        <v>1</v>
+      </c>
       <c r="G15" s="32">
         <v>0</v>
       </c>
-      <c r="BD15" s="46"/>
+      <c r="BD15" s="44"/>
     </row>
     <row r="16" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="22">
@@ -1902,12 +1913,16 @@
       <c r="D16" s="33">
         <v>3</v>
       </c>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
+      <c r="E16" s="33">
+        <v>10</v>
+      </c>
+      <c r="F16" s="33">
+        <v>3</v>
+      </c>
       <c r="G16" s="32">
         <v>0</v>
       </c>
-      <c r="BD16" s="46"/>
+      <c r="BD16" s="44"/>
     </row>
     <row r="17" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22">
@@ -1922,12 +1937,16 @@
       <c r="D17" s="33">
         <v>5</v>
       </c>
-      <c r="E17" s="33"/>
-      <c r="F17" s="33"/>
+      <c r="E17" s="33">
+        <v>13</v>
+      </c>
+      <c r="F17" s="33">
+        <v>3</v>
+      </c>
       <c r="G17" s="32">
         <v>0</v>
       </c>
-      <c r="BD17" s="46"/>
+      <c r="BD17" s="44"/>
     </row>
     <row r="18" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="24" t="s">
@@ -1942,12 +1961,16 @@
       <c r="D18" s="37">
         <v>3</v>
       </c>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
+      <c r="E18" s="37">
+        <v>13</v>
+      </c>
+      <c r="F18" s="37">
+        <v>2</v>
+      </c>
       <c r="G18" s="38">
         <v>0</v>
       </c>
-      <c r="BD18" s="46"/>
+      <c r="BD18" s="44"/>
     </row>
     <row r="19" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="24" t="s">
@@ -1962,12 +1985,16 @@
       <c r="D19" s="37">
         <v>2</v>
       </c>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
+      <c r="E19" s="37">
+        <v>15</v>
+      </c>
+      <c r="F19" s="37">
+        <v>1</v>
+      </c>
       <c r="G19" s="38">
         <v>0</v>
       </c>
-      <c r="BD19" s="46"/>
+      <c r="BD19" s="44"/>
     </row>
     <row r="20" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
@@ -1982,12 +2009,16 @@
       <c r="D20" s="33">
         <v>2</v>
       </c>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
+      <c r="E20" s="33">
+        <v>16</v>
+      </c>
+      <c r="F20" s="33">
+        <v>1</v>
+      </c>
       <c r="G20" s="32">
         <v>0</v>
       </c>
-      <c r="BD20" s="46"/>
+      <c r="BD20" s="44"/>
     </row>
     <row r="21" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20">
@@ -2002,12 +2033,16 @@
       <c r="D21" s="35">
         <v>28</v>
       </c>
-      <c r="E21" s="35"/>
-      <c r="F21" s="35"/>
+      <c r="E21" s="35">
+        <v>15</v>
+      </c>
+      <c r="F21" s="35">
+        <v>30</v>
+      </c>
       <c r="G21" s="36">
         <v>0</v>
       </c>
-      <c r="BD21" s="46"/>
+      <c r="BD21" s="44"/>
     </row>
     <row r="22" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="22">
@@ -2022,12 +2057,16 @@
       <c r="D22" s="33">
         <v>4</v>
       </c>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
+      <c r="E22" s="33">
+        <v>15</v>
+      </c>
+      <c r="F22" s="33">
+        <v>3</v>
+      </c>
       <c r="G22" s="32">
         <v>0</v>
       </c>
-      <c r="BD22" s="46"/>
+      <c r="BD22" s="44"/>
     </row>
     <row r="23" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="22">
@@ -2042,12 +2081,16 @@
       <c r="D23" s="33">
         <v>3</v>
       </c>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
+      <c r="E23" s="33">
+        <v>18</v>
+      </c>
+      <c r="F23" s="33">
+        <v>3</v>
+      </c>
       <c r="G23" s="32">
         <v>0</v>
       </c>
-      <c r="BD23" s="46"/>
+      <c r="BD23" s="44"/>
     </row>
     <row r="24" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="22">
@@ -2062,16 +2105,20 @@
       <c r="D24" s="33">
         <v>5</v>
       </c>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
+      <c r="E24" s="33">
+        <v>31</v>
+      </c>
+      <c r="F24" s="33">
+        <v>3</v>
+      </c>
       <c r="G24" s="32">
         <v>0</v>
       </c>
-      <c r="BD24" s="46"/>
+      <c r="BD24" s="44"/>
     </row>
     <row r="25" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B25" s="25" t="s">
         <v>37</v>
@@ -2082,16 +2129,20 @@
       <c r="D25" s="37">
         <v>3</v>
       </c>
-      <c r="E25" s="37"/>
-      <c r="F25" s="37"/>
+      <c r="E25" s="37">
+        <v>31</v>
+      </c>
+      <c r="F25" s="37">
+        <v>2</v>
+      </c>
       <c r="G25" s="38">
         <v>0</v>
       </c>
-      <c r="BD25" s="46"/>
+      <c r="BD25" s="44"/>
     </row>
     <row r="26" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B26" s="25" t="s">
         <v>38</v>
@@ -2102,12 +2153,16 @@
       <c r="D26" s="37">
         <v>2</v>
       </c>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
+      <c r="E26" s="37">
+        <v>32</v>
+      </c>
+      <c r="F26" s="37">
+        <v>2</v>
+      </c>
       <c r="G26" s="38">
         <v>0</v>
       </c>
-      <c r="BD26" s="46"/>
+      <c r="BD26" s="44"/>
     </row>
     <row r="27" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="22">
@@ -2122,16 +2177,20 @@
       <c r="D27" s="33">
         <v>4</v>
       </c>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
+      <c r="E27" s="33">
+        <v>32</v>
+      </c>
+      <c r="F27" s="33">
+        <v>3</v>
+      </c>
       <c r="G27" s="32">
         <v>0</v>
       </c>
-      <c r="BD27" s="46"/>
+      <c r="BD27" s="44"/>
     </row>
     <row r="28" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B28" s="25" t="s">
         <v>40</v>
@@ -2142,16 +2201,20 @@
       <c r="D28" s="37">
         <v>2</v>
       </c>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
+      <c r="E28" s="37">
+        <v>32</v>
+      </c>
+      <c r="F28" s="37">
+        <v>2</v>
+      </c>
       <c r="G28" s="38">
         <v>0</v>
       </c>
-      <c r="BD28" s="46"/>
+      <c r="BD28" s="44"/>
     </row>
     <row r="29" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B29" s="25" t="s">
         <v>41</v>
@@ -2162,12 +2225,16 @@
       <c r="D29" s="37">
         <v>2</v>
       </c>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
+      <c r="E29" s="37">
+        <v>33</v>
+      </c>
+      <c r="F29" s="37">
+        <v>2</v>
+      </c>
       <c r="G29" s="38">
         <v>0</v>
       </c>
-      <c r="BD29" s="46"/>
+      <c r="BD29" s="44"/>
     </row>
     <row r="30" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="22">
@@ -2182,16 +2249,20 @@
       <c r="D30" s="33">
         <v>4</v>
       </c>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
+      <c r="E30" s="33">
+        <v>35</v>
+      </c>
+      <c r="F30" s="33">
+        <v>8</v>
+      </c>
       <c r="G30" s="32">
         <v>0</v>
       </c>
-      <c r="BD30" s="46"/>
+      <c r="BD30" s="44"/>
     </row>
     <row r="31" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B31" s="25" t="s">
         <v>43</v>
@@ -2202,16 +2273,20 @@
       <c r="D31" s="37">
         <v>2</v>
       </c>
-      <c r="E31" s="37"/>
-      <c r="F31" s="37"/>
+      <c r="E31" s="37">
+        <v>35</v>
+      </c>
+      <c r="F31" s="37">
+        <v>2</v>
+      </c>
       <c r="G31" s="38">
         <v>0</v>
       </c>
-      <c r="BD31" s="46"/>
+      <c r="BD31" s="44"/>
     </row>
     <row r="32" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B32" s="25" t="s">
         <v>44</v>
@@ -2222,16 +2297,20 @@
       <c r="D32" s="37">
         <v>1</v>
       </c>
-      <c r="E32" s="37"/>
-      <c r="F32" s="37"/>
+      <c r="E32" s="37">
+        <v>37</v>
+      </c>
+      <c r="F32" s="37">
+        <v>2</v>
+      </c>
       <c r="G32" s="38">
         <v>0</v>
       </c>
-      <c r="BD32" s="46"/>
+      <c r="BD32" s="44"/>
     </row>
     <row r="33" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B33" s="25" t="s">
         <v>45</v>
@@ -2242,12 +2321,16 @@
       <c r="D33" s="37">
         <v>1</v>
       </c>
-      <c r="E33" s="37"/>
-      <c r="F33" s="37"/>
+      <c r="E33" s="37">
+        <v>39</v>
+      </c>
+      <c r="F33" s="37">
+        <v>4</v>
+      </c>
       <c r="G33" s="38">
         <v>0</v>
       </c>
-      <c r="BD33" s="46"/>
+      <c r="BD33" s="44"/>
     </row>
     <row r="34" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="22">
@@ -2262,16 +2345,20 @@
       <c r="D34" s="33">
         <v>4</v>
       </c>
-      <c r="E34" s="33"/>
-      <c r="F34" s="33"/>
+      <c r="E34" s="33">
+        <v>35</v>
+      </c>
+      <c r="F34" s="33">
+        <v>8</v>
+      </c>
       <c r="G34" s="32">
         <v>0</v>
       </c>
-      <c r="BD34" s="46"/>
+      <c r="BD34" s="44"/>
     </row>
     <row r="35" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B35" s="25" t="s">
         <v>47</v>
@@ -2282,16 +2369,20 @@
       <c r="D35" s="37">
         <v>1</v>
       </c>
-      <c r="E35" s="37"/>
-      <c r="F35" s="37"/>
+      <c r="E35" s="37">
+        <v>35</v>
+      </c>
+      <c r="F35" s="37">
+        <v>1</v>
+      </c>
       <c r="G35" s="38">
         <v>0</v>
       </c>
-      <c r="BD35" s="46"/>
+      <c r="BD35" s="44"/>
     </row>
     <row r="36" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B36" s="25" t="s">
         <v>48</v>
@@ -2302,451 +2393,502 @@
       <c r="D36" s="37">
         <v>2</v>
       </c>
-      <c r="E36" s="37"/>
-      <c r="F36" s="37"/>
+      <c r="E36" s="37">
+        <v>38</v>
+      </c>
+      <c r="F36" s="37">
+        <v>2</v>
+      </c>
       <c r="G36" s="38">
         <v>0</v>
       </c>
-      <c r="BD36" s="46"/>
+      <c r="BD36" s="44"/>
     </row>
     <row r="37" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="B37" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="C37" s="37">
+      <c r="A37" s="22">
+        <v>3.7</v>
+      </c>
+      <c r="B37" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" s="33">
+        <v>32</v>
+      </c>
+      <c r="D37" s="33">
+        <v>4</v>
+      </c>
+      <c r="E37" s="33">
         <v>33</v>
       </c>
-      <c r="D37" s="37">
-        <v>2</v>
-      </c>
-      <c r="E37" s="37"/>
-      <c r="F37" s="37"/>
-      <c r="G37" s="38">
-        <v>0</v>
-      </c>
-      <c r="BD37" s="46"/>
+      <c r="F37" s="33">
+        <v>2</v>
+      </c>
+      <c r="G37" s="32">
+        <v>0</v>
+      </c>
+      <c r="BD37" s="44"/>
     </row>
     <row r="38" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="22">
-        <v>3.7</v>
-      </c>
-      <c r="B38" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="C38" s="33">
+      <c r="A38" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="B38" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" s="37">
         <v>32</v>
       </c>
-      <c r="D38" s="33">
-        <v>4</v>
-      </c>
-      <c r="E38" s="33"/>
-      <c r="F38" s="33"/>
-      <c r="G38" s="32">
-        <v>0</v>
-      </c>
-      <c r="BD38" s="46"/>
+      <c r="D38" s="37">
+        <v>1</v>
+      </c>
+      <c r="E38" s="37">
+        <v>33</v>
+      </c>
+      <c r="F38" s="37">
+        <v>1</v>
+      </c>
+      <c r="G38" s="38">
+        <v>0</v>
+      </c>
+      <c r="BD38" s="44"/>
     </row>
     <row r="39" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B39" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="C39" s="37">
+        <v>45</v>
+      </c>
+      <c r="C39" s="39">
         <v>32</v>
       </c>
-      <c r="D39" s="37">
-        <v>1</v>
-      </c>
-      <c r="E39" s="37"/>
-      <c r="F39" s="37"/>
+      <c r="D39" s="39">
+        <v>2</v>
+      </c>
+      <c r="E39" s="39">
+        <v>34</v>
+      </c>
+      <c r="F39" s="39">
+        <v>2</v>
+      </c>
       <c r="G39" s="38">
         <v>0</v>
       </c>
-      <c r="BD39" s="46"/>
+      <c r="BD39" s="44"/>
     </row>
     <row r="40" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="B40" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40" s="39">
+        <v>33</v>
+      </c>
+      <c r="D40" s="39">
+        <v>2</v>
+      </c>
+      <c r="E40" s="39">
+        <v>35</v>
+      </c>
+      <c r="F40" s="39">
+        <v>1</v>
+      </c>
+      <c r="G40" s="38">
+        <v>0</v>
+      </c>
+      <c r="BD40" s="44"/>
+    </row>
+    <row r="41" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="22">
+        <v>3.8</v>
+      </c>
+      <c r="B41" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C41" s="31">
+        <v>36</v>
+      </c>
+      <c r="D41" s="31">
+        <v>7</v>
+      </c>
+      <c r="E41" s="31">
+        <v>30</v>
+      </c>
+      <c r="F41" s="31">
+        <v>15</v>
+      </c>
+      <c r="G41" s="32">
+        <v>0</v>
+      </c>
+      <c r="BD41" s="44"/>
+    </row>
+    <row r="42" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="B40" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="C40" s="39">
-        <v>32</v>
-      </c>
-      <c r="D40" s="39">
-        <v>2</v>
-      </c>
-      <c r="E40" s="39"/>
-      <c r="F40" s="39"/>
-      <c r="G40" s="38">
-        <v>0</v>
-      </c>
-      <c r="BD40" s="46"/>
-    </row>
-    <row r="41" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="B41" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="C41" s="39">
-        <v>33</v>
-      </c>
-      <c r="D41" s="39">
-        <v>2</v>
-      </c>
-      <c r="E41" s="39"/>
-      <c r="F41" s="39"/>
-      <c r="G41" s="38">
-        <v>0</v>
-      </c>
-      <c r="BD41" s="46"/>
-    </row>
-    <row r="42" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="22">
-        <v>3.8</v>
-      </c>
-      <c r="B42" s="23" t="s">
+      <c r="B42" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="C42" s="31">
+      <c r="C42" s="39">
         <v>36</v>
       </c>
-      <c r="D42" s="31">
-        <v>7</v>
-      </c>
-      <c r="E42" s="31"/>
-      <c r="F42" s="31"/>
-      <c r="G42" s="32">
-        <v>0</v>
-      </c>
-      <c r="BD42" s="46"/>
+      <c r="D42" s="39">
+        <v>4</v>
+      </c>
+      <c r="E42" s="39">
+        <v>37</v>
+      </c>
+      <c r="F42" s="39">
+        <v>8</v>
+      </c>
+      <c r="G42" s="38">
+        <v>0</v>
+      </c>
+      <c r="BD42" s="44"/>
     </row>
     <row r="43" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B43" s="25" t="s">
         <v>52</v>
       </c>
       <c r="C43" s="39">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D43" s="39">
         <v>4</v>
       </c>
-      <c r="E43" s="39"/>
-      <c r="F43" s="39"/>
+      <c r="E43" s="39">
+        <v>30</v>
+      </c>
+      <c r="F43" s="39">
+        <v>8</v>
+      </c>
       <c r="G43" s="38">
         <v>0</v>
       </c>
-      <c r="BD43" s="46"/>
+      <c r="BD43" s="44"/>
     </row>
     <row r="44" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="B44" s="25" t="s">
+      <c r="A44" s="20">
+        <v>4</v>
+      </c>
+      <c r="B44" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="C44" s="39">
-        <v>39</v>
-      </c>
-      <c r="D44" s="39">
+      <c r="C44" s="40">
+        <v>43</v>
+      </c>
+      <c r="D44" s="40">
         <v>4</v>
       </c>
-      <c r="E44" s="39"/>
-      <c r="F44" s="39"/>
-      <c r="G44" s="38">
-        <v>0</v>
-      </c>
-      <c r="BD44" s="46"/>
+      <c r="E44" s="40">
+        <v>45</v>
+      </c>
+      <c r="F44" s="40">
+        <v>4</v>
+      </c>
+      <c r="G44" s="36">
+        <v>0</v>
+      </c>
+      <c r="BD44" s="44"/>
     </row>
     <row r="45" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="20">
-        <v>4</v>
-      </c>
-      <c r="B45" s="21" t="s">
+      <c r="A45" s="22">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B45" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="C45" s="40">
+      <c r="C45" s="31">
         <v>43</v>
       </c>
-      <c r="D45" s="40">
-        <v>4</v>
-      </c>
-      <c r="E45" s="40"/>
-      <c r="F45" s="40"/>
-      <c r="G45" s="36">
-        <v>0</v>
-      </c>
-      <c r="BD45" s="46"/>
+      <c r="D45" s="31">
+        <v>2</v>
+      </c>
+      <c r="E45" s="31">
+        <v>45</v>
+      </c>
+      <c r="F45" s="31">
+        <v>2</v>
+      </c>
+      <c r="G45" s="32">
+        <v>0</v>
+      </c>
+      <c r="BD45" s="44"/>
     </row>
     <row r="46" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="22">
-        <v>4.0999999999999996</v>
+        <v>4.2</v>
       </c>
       <c r="B46" s="23" t="s">
         <v>55</v>
       </c>
       <c r="C46" s="31">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D46" s="31">
-        <v>2</v>
-      </c>
-      <c r="E46" s="31"/>
-      <c r="F46" s="31"/>
+        <v>3</v>
+      </c>
+      <c r="E46" s="31">
+        <v>46</v>
+      </c>
+      <c r="F46" s="31">
+        <v>3</v>
+      </c>
       <c r="G46" s="32">
         <v>0</v>
       </c>
-      <c r="BD46" s="46"/>
+      <c r="BD46" s="44"/>
     </row>
     <row r="47" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="22">
-        <v>4.2</v>
-      </c>
-      <c r="B47" s="23" t="s">
+      <c r="A47" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="B47" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="C47" s="31">
+      <c r="C47" s="39">
         <v>44</v>
       </c>
-      <c r="D47" s="31">
-        <v>3</v>
-      </c>
-      <c r="E47" s="31"/>
-      <c r="F47" s="31"/>
-      <c r="G47" s="32">
-        <v>0</v>
-      </c>
-      <c r="BD47" s="46"/>
+      <c r="D47" s="39">
+        <v>2</v>
+      </c>
+      <c r="E47" s="39">
+        <v>46</v>
+      </c>
+      <c r="F47" s="39">
+        <v>2</v>
+      </c>
+      <c r="G47" s="38">
+        <v>0</v>
+      </c>
+      <c r="BD47" s="44"/>
     </row>
     <row r="48" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B48" s="25" t="s">
         <v>57</v>
       </c>
       <c r="C48" s="39">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D48" s="39">
         <v>2</v>
       </c>
-      <c r="E48" s="39"/>
-      <c r="F48" s="39"/>
+      <c r="E48" s="39">
+        <v>47</v>
+      </c>
+      <c r="F48" s="39">
+        <v>2</v>
+      </c>
       <c r="G48" s="38">
         <v>0</v>
       </c>
-      <c r="BD48" s="46"/>
+      <c r="BD48" s="44"/>
     </row>
     <row r="49" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="B49" s="25" t="s">
+      <c r="A49" s="20">
+        <v>5</v>
+      </c>
+      <c r="B49" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="C49" s="39">
-        <v>45</v>
-      </c>
-      <c r="D49" s="39">
-        <v>2</v>
-      </c>
-      <c r="E49" s="39"/>
-      <c r="F49" s="39"/>
-      <c r="G49" s="38">
-        <v>0</v>
-      </c>
-      <c r="BD49" s="46"/>
+      <c r="C49" s="40">
+        <v>46</v>
+      </c>
+      <c r="D49" s="40">
+        <v>4</v>
+      </c>
+      <c r="E49" s="40">
+        <v>48</v>
+      </c>
+      <c r="F49" s="40">
+        <v>3</v>
+      </c>
+      <c r="G49" s="36">
+        <v>0</v>
+      </c>
+      <c r="BD49" s="44"/>
     </row>
     <row r="50" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="20">
-        <v>5</v>
-      </c>
-      <c r="B50" s="21" t="s">
+      <c r="A50" s="22">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B50" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="C50" s="40">
+      <c r="C50" s="31">
         <v>46</v>
       </c>
-      <c r="D50" s="40">
-        <v>4</v>
-      </c>
-      <c r="E50" s="40"/>
-      <c r="F50" s="40"/>
-      <c r="G50" s="36">
-        <v>0</v>
-      </c>
-      <c r="BD50" s="46"/>
+      <c r="D50" s="31">
+        <v>1</v>
+      </c>
+      <c r="E50" s="31">
+        <v>48</v>
+      </c>
+      <c r="F50" s="31">
+        <v>1</v>
+      </c>
+      <c r="G50" s="32">
+        <v>0</v>
+      </c>
+      <c r="BD50" s="44"/>
     </row>
     <row r="51" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="22">
-        <v>5.0999999999999996</v>
+        <v>5.2</v>
       </c>
       <c r="B51" s="23" t="s">
         <v>60</v>
       </c>
       <c r="C51" s="31">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D51" s="31">
         <v>1</v>
       </c>
-      <c r="E51" s="31"/>
-      <c r="F51" s="31"/>
+      <c r="E51" s="31">
+        <v>49</v>
+      </c>
+      <c r="F51" s="31">
+        <v>1</v>
+      </c>
       <c r="G51" s="32">
         <v>0</v>
       </c>
-      <c r="BD51" s="46"/>
+      <c r="BD51" s="44"/>
     </row>
     <row r="52" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="22">
-        <v>5.2</v>
-      </c>
-      <c r="B52" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C52" s="31">
-        <v>47</v>
-      </c>
-      <c r="D52" s="31">
-        <v>1</v>
-      </c>
-      <c r="E52" s="31"/>
-      <c r="F52" s="31"/>
-      <c r="G52" s="32">
-        <v>0</v>
-      </c>
-      <c r="BD52" s="46"/>
-    </row>
-    <row r="53" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="26">
+      <c r="A52" s="26">
         <v>5.3</v>
       </c>
-      <c r="B53" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="C53" s="41">
+      <c r="B52" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="C52" s="41">
         <v>48</v>
       </c>
-      <c r="D53" s="41">
-        <v>2</v>
-      </c>
-      <c r="E53" s="41"/>
-      <c r="F53" s="41"/>
-      <c r="G53" s="42">
-        <v>0</v>
-      </c>
-      <c r="H53" s="43"/>
-      <c r="I53" s="43"/>
-      <c r="J53" s="43"/>
-      <c r="K53" s="43"/>
-      <c r="L53" s="43"/>
-      <c r="M53" s="43"/>
-      <c r="N53" s="43"/>
-      <c r="O53" s="43"/>
-      <c r="P53" s="43"/>
-      <c r="Q53" s="43"/>
-      <c r="R53" s="43"/>
-      <c r="S53" s="43"/>
-      <c r="T53" s="43"/>
-      <c r="U53" s="43"/>
-      <c r="V53" s="43"/>
-      <c r="W53" s="43"/>
-      <c r="X53" s="43"/>
-      <c r="Y53" s="43"/>
-      <c r="Z53" s="43"/>
-      <c r="AA53" s="43"/>
-      <c r="AB53" s="44"/>
-      <c r="AC53" s="44"/>
-      <c r="AD53" s="44"/>
-      <c r="AE53" s="44"/>
-      <c r="AF53" s="44"/>
-      <c r="AG53" s="44"/>
-      <c r="AH53" s="44"/>
-      <c r="AI53" s="44"/>
-      <c r="AJ53" s="44"/>
-      <c r="AK53" s="44"/>
-      <c r="AL53" s="44"/>
-      <c r="AM53" s="44"/>
-      <c r="AN53" s="44"/>
-      <c r="AO53" s="44"/>
-      <c r="AP53" s="44"/>
-      <c r="AQ53" s="44"/>
-      <c r="AR53" s="44"/>
-      <c r="AS53" s="44"/>
-      <c r="AT53" s="44"/>
-      <c r="AU53" s="44"/>
-      <c r="AV53" s="44"/>
-      <c r="AW53" s="44"/>
-      <c r="AX53" s="44"/>
-      <c r="AY53" s="44"/>
-      <c r="AZ53" s="44"/>
-      <c r="BA53" s="44"/>
-      <c r="BB53" s="44"/>
-      <c r="BC53" s="44"/>
-      <c r="BD53" s="47"/>
+      <c r="D52" s="41">
+        <v>2</v>
+      </c>
+      <c r="E52" s="41">
+        <v>48</v>
+      </c>
+      <c r="F52" s="41">
+        <v>2</v>
+      </c>
+      <c r="G52" s="42">
+        <v>0</v>
+      </c>
+      <c r="BD52" s="44"/>
+    </row>
+    <row r="53" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H53" s="61"/>
+      <c r="I53" s="61"/>
+      <c r="J53" s="61"/>
+      <c r="K53" s="61"/>
+      <c r="L53" s="61"/>
+      <c r="M53" s="61"/>
+      <c r="N53" s="61"/>
+      <c r="O53" s="61"/>
+      <c r="P53" s="61"/>
+      <c r="Q53" s="61"/>
+      <c r="R53" s="61"/>
+      <c r="S53" s="61"/>
+      <c r="T53" s="61"/>
+      <c r="U53" s="61"/>
+      <c r="V53" s="61"/>
+      <c r="W53" s="61"/>
+      <c r="X53" s="61"/>
+      <c r="Y53" s="61"/>
+      <c r="Z53" s="61"/>
+      <c r="AA53" s="61"/>
+      <c r="AB53" s="62"/>
+      <c r="AC53" s="62"/>
+      <c r="AD53" s="62"/>
+      <c r="AE53" s="62"/>
+      <c r="AF53" s="62"/>
+      <c r="AG53" s="62"/>
+      <c r="AH53" s="62"/>
+      <c r="AI53" s="62"/>
+      <c r="AJ53" s="62"/>
+      <c r="AK53" s="62"/>
+      <c r="AL53" s="62"/>
+      <c r="AM53" s="62"/>
+      <c r="AN53" s="62"/>
+      <c r="AO53" s="62"/>
+      <c r="AP53" s="62"/>
+      <c r="AQ53" s="62"/>
+      <c r="AR53" s="62"/>
+      <c r="AS53" s="62"/>
+      <c r="AT53" s="62"/>
+      <c r="AU53" s="62"/>
+      <c r="AV53" s="62"/>
+      <c r="AW53" s="62"/>
+      <c r="AX53" s="62"/>
+      <c r="AY53" s="62"/>
+      <c r="AZ53" s="62"/>
+      <c r="BA53" s="62"/>
+      <c r="BB53" s="62"/>
+      <c r="BC53" s="62"/>
+      <c r="BD53" s="63"/>
     </row>
     <row r="54" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H54" s="48"/>
-      <c r="I54" s="48"/>
-      <c r="J54" s="48"/>
-      <c r="K54" s="48"/>
-      <c r="L54" s="48"/>
-      <c r="M54" s="48"/>
-      <c r="N54" s="48"/>
-      <c r="O54" s="48"/>
-      <c r="P54" s="48"/>
-      <c r="Q54" s="48"/>
-      <c r="R54" s="48"/>
-      <c r="S54" s="48"/>
-      <c r="T54" s="48"/>
-      <c r="U54" s="48"/>
-      <c r="V54" s="48"/>
-      <c r="W54" s="48"/>
-      <c r="X54" s="48"/>
-      <c r="Y54" s="48"/>
-      <c r="Z54" s="48"/>
-      <c r="AA54" s="48"/>
-      <c r="AB54" s="49"/>
-      <c r="AC54" s="49"/>
-      <c r="AD54" s="49"/>
-      <c r="AE54" s="49"/>
-      <c r="AF54" s="49"/>
-      <c r="AG54" s="49"/>
-      <c r="AH54" s="49"/>
-      <c r="AI54" s="49"/>
-      <c r="AJ54" s="49"/>
-      <c r="AK54" s="49"/>
-      <c r="AL54" s="49"/>
-      <c r="AM54" s="49"/>
-      <c r="AN54" s="49"/>
-      <c r="AO54" s="49"/>
-      <c r="AP54" s="49"/>
-      <c r="AQ54" s="49"/>
-      <c r="AR54" s="49"/>
-      <c r="AS54" s="49"/>
-      <c r="AT54" s="49"/>
-      <c r="AU54" s="49"/>
-      <c r="AV54" s="49"/>
-      <c r="AW54" s="49"/>
-      <c r="AX54" s="49"/>
-      <c r="AY54" s="49"/>
-      <c r="AZ54" s="49"/>
-      <c r="BA54" s="49"/>
-      <c r="BB54" s="49"/>
-      <c r="BC54" s="49"/>
-      <c r="BD54" s="49"/>
+      <c r="H54" s="45"/>
+      <c r="I54" s="45"/>
+      <c r="J54" s="45"/>
+      <c r="K54" s="45"/>
+      <c r="L54" s="45"/>
+      <c r="M54" s="45"/>
+      <c r="N54" s="45"/>
+      <c r="O54" s="45"/>
+      <c r="P54" s="45"/>
+      <c r="Q54" s="45"/>
+      <c r="R54" s="45"/>
+      <c r="S54" s="45"/>
+      <c r="T54" s="45"/>
+      <c r="U54" s="45"/>
+      <c r="V54" s="45"/>
+      <c r="W54" s="45"/>
+      <c r="X54" s="45"/>
+      <c r="Y54" s="45"/>
+      <c r="Z54" s="45"/>
+      <c r="AA54" s="45"/>
+      <c r="AB54" s="46"/>
+      <c r="AC54" s="46"/>
+      <c r="AD54" s="46"/>
+      <c r="AE54" s="46"/>
+      <c r="AF54" s="46"/>
+      <c r="AG54" s="46"/>
+      <c r="AH54" s="46"/>
+      <c r="AI54" s="46"/>
+      <c r="AJ54" s="46"/>
+      <c r="AK54" s="46"/>
+      <c r="AL54" s="46"/>
+      <c r="AM54" s="46"/>
+      <c r="AN54" s="46"/>
+      <c r="AO54" s="46"/>
+      <c r="AP54" s="46"/>
+      <c r="AQ54" s="46"/>
+      <c r="AR54" s="46"/>
+      <c r="AS54" s="46"/>
+      <c r="AT54" s="46"/>
+      <c r="AU54" s="46"/>
+      <c r="AV54" s="46"/>
+      <c r="AW54" s="46"/>
+      <c r="AX54" s="46"/>
+      <c r="AY54" s="46"/>
+      <c r="AZ54" s="46"/>
+      <c r="BA54" s="46"/>
+      <c r="BB54" s="46"/>
+      <c r="BC54" s="46"/>
+      <c r="BD54" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -2762,35 +2904,35 @@
     <mergeCell ref="V2:Y2"/>
     <mergeCell ref="AA2:AG2"/>
   </mergeCells>
+  <conditionalFormatting sqref="H4:BO4">
+    <cfRule type="expression" dxfId="8" priority="8">
+      <formula>H$4=period_selected</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="H5:BO53">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="3">
+    <cfRule type="expression" dxfId="6" priority="3">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="4">
+    <cfRule type="expression" dxfId="5" priority="4">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="3" priority="6">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="7">
+    <cfRule type="expression" dxfId="2" priority="7">
       <formula>H$4=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="11">
+    <cfRule type="expression" dxfId="1" priority="11">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="12">
+    <cfRule type="expression" dxfId="0" priority="12">
       <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H4:BO4">
-    <cfRule type="expression" dxfId="0" priority="8">
-      <formula>H$4=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="16">

</xml_diff>